<commit_message>
keleta klausimu pasiulymu i exeliuka, kad nepamirst
</commit_message>
<xml_diff>
--- a/01_dokumentacija/JUDALABIAU_bugs_v0.01.xlsx
+++ b/01_dokumentacija/JUDALABIAU_bugs_v0.01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19222"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11D6FE71-6904-4058-91DF-89887A6DFA29}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="klausimai" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,24 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Tema</t>
+  </si>
+  <si>
     <t>Plačiau apie vabalą/klausimas aptarimui</t>
   </si>
   <si>
-    <t>Tema</t>
-  </si>
-  <si>
     <t>Open/Closed</t>
+  </si>
+  <si>
+    <t>.idea fronete? webstormo bajeriai ar missclickas</t>
+  </si>
+  <si>
+    <t>node_modules pabego 3 moduliai is fronto, webstrom prikolas ar missclickas?</t>
+  </si>
+  <si>
+    <t>siulau db kataloga kist i doc</t>
+  </si>
+  <si>
+    <t>paveldejimas, viena didele su daug nulu kur kam nepriklauso laukai ar paveldinti savo lentele? kolkas padaryat paveldinti savo</t>
+  </si>
+  <si>
+    <t>del medzio, userius siulau viduj palikt tris katalogus nes nebus vieno serviso vieno kontrolerio tiesiog useriui, ar bus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -196,6 +212,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -242,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,9 +298,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,6 +350,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,14 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AML3"/>
+  <dimension ref="A1:AML6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -507,10 +567,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -520,14 +580,33 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>